<commit_message>
updated by week 3 - class 6
</commit_message>
<xml_diff>
--- a/TrackAttendance.xlsx
+++ b/TrackAttendance.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tam2\Dropbox\GithubProjects\TrackME2024Attendance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tam2\Dropbox\Trabalho\DBA\2024_2025\ME2024\Notas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6A11555-C433-4D71-99D1-9FDB47365520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9E326D-39F7-4597-81D8-984D52060A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-51720" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -136,12 +136,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -156,9 +162,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +490,7 @@
   <dimension ref="A1:Y49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Y49"/>
+      <selection activeCell="AD22" sqref="AD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -582,10 +589,10 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -736,10 +743,10 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -816,7 +823,7 @@
         <v>0</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -887,13 +894,13 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -967,10 +974,10 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1044,10 +1051,10 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1121,10 +1128,10 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1198,10 +1205,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1275,10 +1282,10 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1355,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1429,7 +1436,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1506,10 +1513,10 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -1583,10 +1590,10 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -1660,10 +1667,10 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -1737,10 +1744,10 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -1814,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1888,13 +1895,13 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1968,10 +1975,10 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -2045,10 +2052,10 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -2122,7 +2129,7 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -2199,10 +2206,10 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -2276,10 +2283,10 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -2356,7 +2363,7 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -2430,10 +2437,10 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -2507,10 +2514,10 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -2584,10 +2591,10 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -2661,10 +2668,10 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -2738,10 +2745,10 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -2815,10 +2822,10 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -2892,10 +2899,10 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -2969,10 +2976,10 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -3046,10 +3053,10 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -3123,10 +3130,10 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -3200,10 +3207,10 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -3274,13 +3281,13 @@
         <v>1</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -3354,10 +3361,10 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -3431,10 +3438,10 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -3508,10 +3515,10 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -3585,7 +3592,7 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -3662,10 +3669,10 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -3739,10 +3746,10 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -3803,76 +3810,76 @@
       <c r="A44" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="J44">
-        <v>0</v>
-      </c>
-      <c r="K44">
-        <v>0</v>
-      </c>
-      <c r="L44">
-        <v>0</v>
-      </c>
-      <c r="M44">
-        <v>0</v>
-      </c>
-      <c r="N44">
-        <v>0</v>
-      </c>
-      <c r="O44">
-        <v>0</v>
-      </c>
-      <c r="P44">
-        <v>0</v>
-      </c>
-      <c r="Q44">
-        <v>0</v>
-      </c>
-      <c r="R44">
-        <v>0</v>
-      </c>
-      <c r="S44">
-        <v>0</v>
-      </c>
-      <c r="T44">
-        <v>0</v>
-      </c>
-      <c r="U44">
-        <v>0</v>
-      </c>
-      <c r="V44">
-        <v>0</v>
-      </c>
-      <c r="W44">
-        <v>0</v>
-      </c>
-      <c r="X44">
-        <v>0</v>
-      </c>
-      <c r="Y44">
+      <c r="B44" s="2">
+        <v>0</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0</v>
+      </c>
+      <c r="I44" s="2">
+        <v>0</v>
+      </c>
+      <c r="J44" s="2">
+        <v>0</v>
+      </c>
+      <c r="K44" s="2">
+        <v>0</v>
+      </c>
+      <c r="L44" s="2">
+        <v>0</v>
+      </c>
+      <c r="M44" s="2">
+        <v>0</v>
+      </c>
+      <c r="N44" s="2">
+        <v>0</v>
+      </c>
+      <c r="O44" s="2">
+        <v>0</v>
+      </c>
+      <c r="P44" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>0</v>
+      </c>
+      <c r="R44" s="2">
+        <v>0</v>
+      </c>
+      <c r="S44" s="2">
+        <v>0</v>
+      </c>
+      <c r="T44" s="2">
+        <v>0</v>
+      </c>
+      <c r="U44" s="2">
+        <v>0</v>
+      </c>
+      <c r="V44" s="2">
+        <v>0</v>
+      </c>
+      <c r="W44" s="2">
+        <v>0</v>
+      </c>
+      <c r="X44" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="2">
         <v>0</v>
       </c>
     </row>
@@ -3893,10 +3900,10 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -3967,13 +3974,13 @@
         <v>1</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -4047,7 +4054,7 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -4124,10 +4131,10 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -4201,10 +4208,10 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
         <v>0</v>

</xml_diff>